<commit_message>
reformatted dates in the data file.
</commit_message>
<xml_diff>
--- a/inst/file.xlsx
+++ b/inst/file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\decicco1\OneDrive - Michigan State University\CSTATRedirects\Documents\R Studio Projects\AARUG_Presentation_2022_12_15_Parameters\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9807EF99-4877-464A-A930-C5CE0FEE6EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8327D8-FED3-4338-BC9C-A7C3B19CCBB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2832" yWindow="0" windowWidth="20304" windowHeight="11652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,6 +73,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -104,7 +107,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -164,7 +167,7 @@
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$37</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>yyyy\-mm\-dd;@</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
                   <c:v>43831</c:v>
@@ -284,112 +287,112 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
-                  <c:v>3.670809583302777</c:v>
+                  <c:v>3.9685916677345876</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0930886696286954</c:v>
+                  <c:v>3.497817523523552</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.3409634730106137</c:v>
+                  <c:v>3.0582168408884698</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2237911454614456</c:v>
+                  <c:v>1.7162204864588979</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5917433280492399</c:v>
+                  <c:v>1.5095822526892153</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1280796389245706</c:v>
+                  <c:v>1.9960393933418474</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2303584504699674</c:v>
+                  <c:v>1.2560115149363091</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4873423273143329</c:v>
+                  <c:v>1.9974144769847371</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.3942356283299913</c:v>
+                  <c:v>1.935338577491919</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.570990719118619</c:v>
+                  <c:v>2.2311926552171721</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.8084263258738948</c:v>
+                  <c:v>2.7409891442730907</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.9007835046750929</c:v>
+                  <c:v>2.6849532221830721</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.554237215703556</c:v>
+                  <c:v>3.6770573897592334</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.662059869312877</c:v>
+                  <c:v>3.5809737650706763</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.7908309271352225</c:v>
+                  <c:v>3.2237347751089231</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.5566706954616538</c:v>
+                  <c:v>1.8316236762796509</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.9623513169843492</c:v>
+                  <c:v>1.5118194297960481</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.4566775946780668</c:v>
+                  <c:v>1.5031234651448266</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.0728279467004551</c:v>
+                  <c:v>1.9566535507997782</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.4742657365456555</c:v>
+                  <c:v>1.0416144943535701</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.8997322185647474</c:v>
+                  <c:v>1.4785341565685495</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.002404574239375</c:v>
+                  <c:v>2.803830106581779</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.8445584159366955</c:v>
+                  <c:v>2.4562496969929151</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.9406908109035497</c:v>
+                  <c:v>2.4671184424994292</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.9230776283414768</c:v>
+                  <c:v>3.2324298346484941</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.4554380132151929</c:v>
+                  <c:v>3.8821765041512775</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.5705220501281993</c:v>
+                  <c:v>3.0603146254777354</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.455045252684505</c:v>
+                  <c:v>1.1423862999946022</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.2953782701215244</c:v>
+                  <c:v>1.9772633105802251</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.0520766488117061</c:v>
+                  <c:v>1.6247910030749004</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.100366151843255</c:v>
+                  <c:v>1.332051587015765</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.7920038552830384</c:v>
+                  <c:v>1.7500616282879111</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.4485238988340963</c:v>
+                  <c:v>1.7449105380502865</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.9684010300274117</c:v>
+                  <c:v>2.196255549279674</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.4135731385451673</c:v>
+                  <c:v>2.9784623391988001</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.746815662363058</c:v>
+                  <c:v>2.1767115010322078</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -423,7 +426,7 @@
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$37</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>yyyy\-mm\-dd;@</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
                   <c:v>43831</c:v>
@@ -543,112 +546,112 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
-                  <c:v>2.6989982900564451</c:v>
+                  <c:v>2.0347217454507787</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.651311161386638</c:v>
+                  <c:v>2.5023887509893874</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.6132383583386822</c:v>
+                  <c:v>2.6334896271036121</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.78741059256498991</c:v>
+                  <c:v>0.89834917107120338</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.94141588295523615</c:v>
+                  <c:v>0.30355099534848617</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.27483567609806281</c:v>
+                  <c:v>0.76312192205773055</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.23542039292060346</c:v>
+                  <c:v>0.29197134504691857</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.15686851487223319</c:v>
+                  <c:v>0.43054534337404393</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.49211762619827437</c:v>
+                  <c:v>8.1946656076618885E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.3560733732273436</c:v>
+                  <c:v>2.8964371525828359</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.2170807117418221</c:v>
+                  <c:v>2.0317419180576732</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.7915820659544623</c:v>
+                  <c:v>2.0304721003128203</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.4450497150401733</c:v>
+                  <c:v>2.2005759903003228</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.6824761163846493</c:v>
+                  <c:v>2.5223536220866007</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.3746349081997509</c:v>
+                  <c:v>2.4798385840768091</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.12066079565890253</c:v>
+                  <c:v>0.77195167817096844</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.7402261013506376</c:v>
+                  <c:v>0.15115754224852285</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.59840612245510938</c:v>
+                  <c:v>0.1308136126154289</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.45218468174951487</c:v>
+                  <c:v>0.52735043157173811</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.29656183889152232</c:v>
+                  <c:v>0.7015579341649063</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.8034472312355367E-2</c:v>
+                  <c:v>0.54241414212575956</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.4138596602646416</c:v>
+                  <c:v>2.15081201508931</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.3081442471691407</c:v>
+                  <c:v>2.9782877681928568</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.7097344613680532</c:v>
+                  <c:v>2.8775550816594277</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.9774161730362438</c:v>
+                  <c:v>2.2866393659277877</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.8326475120520795</c:v>
+                  <c:v>2.6562140164435228</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.6871575410467408</c:v>
+                  <c:v>2.7437078573638143</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.33226130385307395</c:v>
+                  <c:v>0.53034549461795277</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.96681640820509573</c:v>
+                  <c:v>0.94533663534186496</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.93076280053761484</c:v>
+                  <c:v>0.48250393374354528</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>5.1959462495823949E-2</c:v>
+                  <c:v>0.21978252295276735</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.92422374275418029</c:v>
+                  <c:v>0.96040532516298127</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.56148099198997736</c:v>
+                  <c:v>0.74185692114156843</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.2032332439296143</c:v>
+                  <c:v>2.8704030592869625</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.75041547329289</c:v>
+                  <c:v>2.1154943756593414</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.3355831804449991</c:v>
+                  <c:v>2.3972645233715055</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -679,7 +682,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="yyyy\-mm\-dd;@" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1721,7 +1724,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A73"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -1770,7 +1775,7 @@
       </c>
       <c r="D2">
         <f t="array" ref="D2:D73" ca="1">RAND()</f>
-        <v>0.67080958330277718</v>
+        <v>0.96859166773458771</v>
       </c>
       <c r="E2">
         <f>IF(B2="Europe",1,0)</f>
@@ -1786,7 +1791,7 @@
       </c>
       <c r="H2">
         <f ca="1">SUM(D2:G2)</f>
-        <v>3.670809583302777</v>
+        <v>3.9685916677345876</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1802,7 +1807,7 @@
       </c>
       <c r="D3">
         <f ca="1"/>
-        <v>9.3088669628695664E-2</v>
+        <v>0.4978175235235518</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E66" si="1">IF(B3="Europe",1,0)</f>
@@ -1818,7 +1823,7 @@
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H66" ca="1" si="4">SUM(D3:G3)</f>
-        <v>3.0930886696286954</v>
+        <v>3.497817523523552</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1834,7 +1839,7 @@
       </c>
       <c r="D4">
         <f ca="1"/>
-        <v>0.34096347301061369</v>
+        <v>5.8216840888469568E-2</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
@@ -1850,7 +1855,7 @@
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="4"/>
-        <v>3.3409634730106137</v>
+        <v>3.0582168408884698</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1866,7 +1871,7 @@
       </c>
       <c r="D5">
         <f ca="1"/>
-        <v>0.22379114546144563</v>
+        <v>0.7162204864588978</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
@@ -1882,7 +1887,7 @@
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="4"/>
-        <v>1.2237911454614456</v>
+        <v>1.7162204864588979</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1898,7 +1903,7 @@
       </c>
       <c r="D6">
         <f ca="1"/>
-        <v>0.59174332804923979</v>
+        <v>0.5095822526892152</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
@@ -1914,7 +1919,7 @@
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="4"/>
-        <v>1.5917433280492399</v>
+        <v>1.5095822526892153</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1930,7 +1935,7 @@
       </c>
       <c r="D7">
         <f ca="1"/>
-        <v>0.12807963892457075</v>
+        <v>0.99603939334184743</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
@@ -1946,7 +1951,7 @@
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="4"/>
-        <v>1.1280796389245706</v>
+        <v>1.9960393933418474</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1962,7 +1967,7 @@
       </c>
       <c r="D8">
         <f ca="1"/>
-        <v>0.23035845046996728</v>
+        <v>0.25601151493630914</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
@@ -1978,7 +1983,7 @@
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="4"/>
-        <v>1.2303584504699674</v>
+        <v>1.2560115149363091</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1994,7 +1999,7 @@
       </c>
       <c r="D9">
         <f ca="1"/>
-        <v>0.48734232731433291</v>
+        <v>0.99741447698473717</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
@@ -2010,7 +2015,7 @@
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="4"/>
-        <v>1.4873423273143329</v>
+        <v>1.9974144769847371</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2026,7 +2031,7 @@
       </c>
       <c r="D10">
         <f ca="1"/>
-        <v>0.39423562832999137</v>
+        <v>0.93533857749191907</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
@@ -2042,7 +2047,7 @@
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="4"/>
-        <v>1.3942356283299913</v>
+        <v>1.935338577491919</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2058,7 +2063,7 @@
       </c>
       <c r="D11">
         <f ca="1"/>
-        <v>0.57099071911861898</v>
+        <v>0.23119265521717214</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
@@ -2074,7 +2079,7 @@
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="4"/>
-        <v>2.570990719118619</v>
+        <v>2.2311926552171721</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2090,7 +2095,7 @@
       </c>
       <c r="D12">
         <f ca="1"/>
-        <v>0.80842632587389474</v>
+        <v>0.74098914427309071</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
@@ -2106,7 +2111,7 @@
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="4"/>
-        <v>2.8084263258738948</v>
+        <v>2.7409891442730907</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2122,7 +2127,7 @@
       </c>
       <c r="D13">
         <f ca="1"/>
-        <v>0.90078350467509305</v>
+        <v>0.6849532221830722</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
@@ -2138,7 +2143,7 @@
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="4"/>
-        <v>2.9007835046750929</v>
+        <v>2.6849532221830721</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2154,7 +2159,7 @@
       </c>
       <c r="D14">
         <f ca="1"/>
-        <v>0.55423721570355611</v>
+        <v>0.67705738975923324</v>
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
@@ -2170,7 +2175,7 @@
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="4"/>
-        <v>3.554237215703556</v>
+        <v>3.6770573897592334</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2186,7 +2191,7 @@
       </c>
       <c r="D15">
         <f ca="1"/>
-        <v>0.66205986931287708</v>
+        <v>0.58097376507067644</v>
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
@@ -2202,7 +2207,7 @@
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="4"/>
-        <v>3.662059869312877</v>
+        <v>3.5809737650706763</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2218,7 +2223,7 @@
       </c>
       <c r="D16">
         <f ca="1"/>
-        <v>0.79083092713522252</v>
+        <v>0.22373477510892326</v>
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
@@ -2234,7 +2239,7 @@
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="4"/>
-        <v>3.7908309271352225</v>
+        <v>3.2237347751089231</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2250,7 +2255,7 @@
       </c>
       <c r="D17">
         <f ca="1"/>
-        <v>0.55667069546165382</v>
+        <v>0.83162367627965106</v>
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
@@ -2266,7 +2271,7 @@
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="4"/>
-        <v>1.5566706954616538</v>
+        <v>1.8316236762796509</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2282,7 +2287,7 @@
       </c>
       <c r="D18">
         <f ca="1"/>
-        <v>0.96235131698434917</v>
+        <v>0.511819429796048</v>
       </c>
       <c r="E18">
         <f t="shared" si="1"/>
@@ -2298,7 +2303,7 @@
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="4"/>
-        <v>1.9623513169843492</v>
+        <v>1.5118194297960481</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2314,7 +2319,7 @@
       </c>
       <c r="D19">
         <f ca="1"/>
-        <v>0.45667759467806679</v>
+        <v>0.50312346514482664</v>
       </c>
       <c r="E19">
         <f t="shared" si="1"/>
@@ -2330,7 +2335,7 @@
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="4"/>
-        <v>1.4566775946780668</v>
+        <v>1.5031234651448266</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2346,7 +2351,7 @@
       </c>
       <c r="D20">
         <f ca="1"/>
-        <v>7.2827946700455004E-2</v>
+        <v>0.95665355079977821</v>
       </c>
       <c r="E20">
         <f t="shared" si="1"/>
@@ -2362,7 +2367,7 @@
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="4"/>
-        <v>1.0728279467004551</v>
+        <v>1.9566535507997782</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2378,7 +2383,7 @@
       </c>
       <c r="D21">
         <f ca="1"/>
-        <v>0.4742657365456554</v>
+        <v>4.1614494353570231E-2</v>
       </c>
       <c r="E21">
         <f t="shared" si="1"/>
@@ -2394,7 +2399,7 @@
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="4"/>
-        <v>1.4742657365456555</v>
+        <v>1.0416144943535701</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2410,7 +2415,7 @@
       </c>
       <c r="D22">
         <f ca="1"/>
-        <v>0.89973221856474728</v>
+        <v>0.47853415656854936</v>
       </c>
       <c r="E22">
         <f t="shared" si="1"/>
@@ -2426,7 +2431,7 @@
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="4"/>
-        <v>1.8997322185647474</v>
+        <v>1.4785341565685495</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2442,7 +2447,7 @@
       </c>
       <c r="D23">
         <f ca="1"/>
-        <v>2.4045742393749014E-3</v>
+        <v>0.80383010658177889</v>
       </c>
       <c r="E23">
         <f t="shared" si="1"/>
@@ -2458,7 +2463,7 @@
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="4"/>
-        <v>2.002404574239375</v>
+        <v>2.803830106581779</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2474,7 +2479,7 @@
       </c>
       <c r="D24">
         <f ca="1"/>
-        <v>0.84455841593669545</v>
+        <v>0.45624969699291495</v>
       </c>
       <c r="E24">
         <f t="shared" si="1"/>
@@ -2490,7 +2495,7 @@
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="4"/>
-        <v>2.8445584159366955</v>
+        <v>2.4562496969929151</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2506,7 +2511,7 @@
       </c>
       <c r="D25">
         <f ca="1"/>
-        <v>0.94069081090354956</v>
+        <v>0.46711844249942902</v>
       </c>
       <c r="E25">
         <f t="shared" si="1"/>
@@ -2522,7 +2527,7 @@
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="4"/>
-        <v>2.9406908109035497</v>
+        <v>2.4671184424994292</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2538,7 +2543,7 @@
       </c>
       <c r="D26">
         <f ca="1"/>
-        <v>0.92307762834147689</v>
+        <v>0.23242983464849432</v>
       </c>
       <c r="E26">
         <f t="shared" si="1"/>
@@ -2554,7 +2559,7 @@
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="4"/>
-        <v>3.9230776283414768</v>
+        <v>3.2324298346484941</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2570,7 +2575,7 @@
       </c>
       <c r="D27">
         <f ca="1"/>
-        <v>0.45543801321519306</v>
+        <v>0.88217650415127746</v>
       </c>
       <c r="E27">
         <f t="shared" si="1"/>
@@ -2586,7 +2591,7 @@
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="4"/>
-        <v>3.4554380132151929</v>
+        <v>3.8821765041512775</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2602,7 +2607,7 @@
       </c>
       <c r="D28">
         <f ca="1"/>
-        <v>0.57052205012819923</v>
+        <v>6.0314625477735584E-2</v>
       </c>
       <c r="E28">
         <f t="shared" si="1"/>
@@ -2618,7 +2623,7 @@
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="4"/>
-        <v>3.5705220501281993</v>
+        <v>3.0603146254777354</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2634,7 +2639,7 @@
       </c>
       <c r="D29">
         <f ca="1"/>
-        <v>0.45504525268450502</v>
+        <v>0.14238629999460228</v>
       </c>
       <c r="E29">
         <f t="shared" si="1"/>
@@ -2650,7 +2655,7 @@
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="4"/>
-        <v>1.455045252684505</v>
+        <v>1.1423862999946022</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2666,7 +2671,7 @@
       </c>
       <c r="D30">
         <f ca="1"/>
-        <v>0.2953782701215244</v>
+        <v>0.97726331058022509</v>
       </c>
       <c r="E30">
         <f t="shared" si="1"/>
@@ -2682,7 +2687,7 @@
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="4"/>
-        <v>1.2953782701215244</v>
+        <v>1.9772633105802251</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2698,7 +2703,7 @@
       </c>
       <c r="D31">
         <f ca="1"/>
-        <v>5.2076648811706039E-2</v>
+        <v>0.62479100307490054</v>
       </c>
       <c r="E31">
         <f t="shared" si="1"/>
@@ -2714,7 +2719,7 @@
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="4"/>
-        <v>1.0520766488117061</v>
+        <v>1.6247910030749004</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2730,7 +2735,7 @@
       </c>
       <c r="D32">
         <f ca="1"/>
-        <v>0.10036615184325492</v>
+        <v>0.33205158701576498</v>
       </c>
       <c r="E32">
         <f t="shared" si="1"/>
@@ -2746,7 +2751,7 @@
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="4"/>
-        <v>1.100366151843255</v>
+        <v>1.332051587015765</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2762,7 +2767,7 @@
       </c>
       <c r="D33">
         <f ca="1"/>
-        <v>0.7920038552830384</v>
+        <v>0.75006162828791123</v>
       </c>
       <c r="E33">
         <f t="shared" si="1"/>
@@ -2778,7 +2783,7 @@
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="4"/>
-        <v>1.7920038552830384</v>
+        <v>1.7500616282879111</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2794,7 +2799,7 @@
       </c>
       <c r="D34">
         <f ca="1"/>
-        <v>0.44852389883409627</v>
+        <v>0.74491053805028662</v>
       </c>
       <c r="E34">
         <f t="shared" si="1"/>
@@ -2810,7 +2815,7 @@
       </c>
       <c r="H34">
         <f t="shared" ca="1" si="4"/>
-        <v>1.4485238988340963</v>
+        <v>1.7449105380502865</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2826,7 +2831,7 @@
       </c>
       <c r="D35">
         <f ca="1"/>
-        <v>0.96840103002741162</v>
+        <v>0.19625554927967381</v>
       </c>
       <c r="E35">
         <f t="shared" si="1"/>
@@ -2842,7 +2847,7 @@
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="4"/>
-        <v>2.9684010300274117</v>
+        <v>2.196255549279674</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2858,7 +2863,7 @@
       </c>
       <c r="D36">
         <f ca="1"/>
-        <v>0.41357313854516742</v>
+        <v>0.9784623391988001</v>
       </c>
       <c r="E36">
         <f t="shared" si="1"/>
@@ -2874,7 +2879,7 @@
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="4"/>
-        <v>2.4135731385451673</v>
+        <v>2.9784623391988001</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2890,7 +2895,7 @@
       </c>
       <c r="D37">
         <f ca="1"/>
-        <v>0.74681566236305796</v>
+        <v>0.17671150103220767</v>
       </c>
       <c r="E37">
         <f t="shared" si="1"/>
@@ -2906,7 +2911,7 @@
       </c>
       <c r="H37">
         <f t="shared" ca="1" si="4"/>
-        <v>2.746815662363058</v>
+        <v>2.1767115010322078</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2922,7 +2927,7 @@
       </c>
       <c r="D38">
         <f ca="1"/>
-        <v>0.69899829005644509</v>
+        <v>3.4721745450778441E-2</v>
       </c>
       <c r="E38">
         <f t="shared" si="1"/>
@@ -2938,7 +2943,7 @@
       </c>
       <c r="H38">
         <f t="shared" ca="1" si="4"/>
-        <v>2.6989982900564451</v>
+        <v>2.0347217454507787</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2954,7 +2959,7 @@
       </c>
       <c r="D39">
         <f ca="1"/>
-        <v>0.65131116138663803</v>
+        <v>0.5023887509893874</v>
       </c>
       <c r="E39">
         <f t="shared" si="1"/>
@@ -2970,7 +2975,7 @@
       </c>
       <c r="H39">
         <f t="shared" ca="1" si="4"/>
-        <v>2.651311161386638</v>
+        <v>2.5023887509893874</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2986,7 +2991,7 @@
       </c>
       <c r="D40">
         <f ca="1"/>
-        <v>0.61323835833868234</v>
+        <v>0.63348962710361223</v>
       </c>
       <c r="E40">
         <f t="shared" si="1"/>
@@ -3002,7 +3007,7 @@
       </c>
       <c r="H40">
         <f t="shared" ca="1" si="4"/>
-        <v>2.6132383583386822</v>
+        <v>2.6334896271036121</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3018,7 +3023,7 @@
       </c>
       <c r="D41">
         <f ca="1"/>
-        <v>0.78741059256498991</v>
+        <v>0.89834917107120338</v>
       </c>
       <c r="E41">
         <f t="shared" si="1"/>
@@ -3034,7 +3039,7 @@
       </c>
       <c r="H41">
         <f t="shared" ca="1" si="4"/>
-        <v>0.78741059256498991</v>
+        <v>0.89834917107120338</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3050,7 +3055,7 @@
       </c>
       <c r="D42">
         <f ca="1"/>
-        <v>0.94141588295523615</v>
+        <v>0.30355099534848617</v>
       </c>
       <c r="E42">
         <f t="shared" si="1"/>
@@ -3066,7 +3071,7 @@
       </c>
       <c r="H42">
         <f t="shared" ca="1" si="4"/>
-        <v>0.94141588295523615</v>
+        <v>0.30355099534848617</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3082,7 +3087,7 @@
       </c>
       <c r="D43">
         <f ca="1"/>
-        <v>0.27483567609806281</v>
+        <v>0.76312192205773055</v>
       </c>
       <c r="E43">
         <f t="shared" si="1"/>
@@ -3098,7 +3103,7 @@
       </c>
       <c r="H43">
         <f t="shared" ca="1" si="4"/>
-        <v>0.27483567609806281</v>
+        <v>0.76312192205773055</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3114,7 +3119,7 @@
       </c>
       <c r="D44">
         <f ca="1"/>
-        <v>0.23542039292060346</v>
+        <v>0.29197134504691857</v>
       </c>
       <c r="E44">
         <f t="shared" si="1"/>
@@ -3130,7 +3135,7 @@
       </c>
       <c r="H44">
         <f t="shared" ca="1" si="4"/>
-        <v>0.23542039292060346</v>
+        <v>0.29197134504691857</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3146,7 +3151,7 @@
       </c>
       <c r="D45">
         <f ca="1"/>
-        <v>0.15686851487223319</v>
+        <v>0.43054534337404393</v>
       </c>
       <c r="E45">
         <f t="shared" si="1"/>
@@ -3162,7 +3167,7 @@
       </c>
       <c r="H45">
         <f t="shared" ca="1" si="4"/>
-        <v>0.15686851487223319</v>
+        <v>0.43054534337404393</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3178,7 +3183,7 @@
       </c>
       <c r="D46">
         <f ca="1"/>
-        <v>0.49211762619827437</v>
+        <v>8.1946656076618885E-2</v>
       </c>
       <c r="E46">
         <f t="shared" si="1"/>
@@ -3194,7 +3199,7 @@
       </c>
       <c r="H46">
         <f t="shared" ca="1" si="4"/>
-        <v>0.49211762619827437</v>
+        <v>8.1946656076618885E-2</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3210,7 +3215,7 @@
       </c>
       <c r="D47">
         <f ca="1"/>
-        <v>0.35607337322734356</v>
+        <v>0.89643715258283607</v>
       </c>
       <c r="E47">
         <f t="shared" si="1"/>
@@ -3226,7 +3231,7 @@
       </c>
       <c r="H47">
         <f t="shared" ca="1" si="4"/>
-        <v>2.3560733732273436</v>
+        <v>2.8964371525828359</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3242,7 +3247,7 @@
       </c>
       <c r="D48">
         <f ca="1"/>
-        <v>0.21708071174182186</v>
+        <v>3.1741918057673235E-2</v>
       </c>
       <c r="E48">
         <f t="shared" si="1"/>
@@ -3258,7 +3263,7 @@
       </c>
       <c r="H48">
         <f t="shared" ca="1" si="4"/>
-        <v>2.2170807117418221</v>
+        <v>2.0317419180576732</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3274,7 +3279,7 @@
       </c>
       <c r="D49">
         <f ca="1"/>
-        <v>0.79158206595446212</v>
+        <v>3.0472100312820327E-2</v>
       </c>
       <c r="E49">
         <f t="shared" si="1"/>
@@ -3290,7 +3295,7 @@
       </c>
       <c r="H49">
         <f t="shared" ca="1" si="4"/>
-        <v>2.7915820659544623</v>
+        <v>2.0304721003128203</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3306,7 +3311,7 @@
       </c>
       <c r="D50">
         <f ca="1"/>
-        <v>0.44504971504017332</v>
+        <v>0.20057599030032291</v>
       </c>
       <c r="E50">
         <f t="shared" si="1"/>
@@ -3322,7 +3327,7 @@
       </c>
       <c r="H50">
         <f t="shared" ca="1" si="4"/>
-        <v>2.4450497150401733</v>
+        <v>2.2005759903003228</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3338,7 +3343,7 @@
       </c>
       <c r="D51">
         <f ca="1"/>
-        <v>0.68247611638464933</v>
+        <v>0.52235362208660086</v>
       </c>
       <c r="E51">
         <f t="shared" si="1"/>
@@ -3354,7 +3359,7 @@
       </c>
       <c r="H51">
         <f t="shared" ca="1" si="4"/>
-        <v>2.6824761163846493</v>
+        <v>2.5223536220866007</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3370,7 +3375,7 @@
       </c>
       <c r="D52">
         <f ca="1"/>
-        <v>0.37463490819975098</v>
+        <v>0.47983858407680902</v>
       </c>
       <c r="E52">
         <f t="shared" si="1"/>
@@ -3386,7 +3391,7 @@
       </c>
       <c r="H52">
         <f t="shared" ca="1" si="4"/>
-        <v>2.3746349081997509</v>
+        <v>2.4798385840768091</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3402,7 +3407,7 @@
       </c>
       <c r="D53">
         <f ca="1"/>
-        <v>0.12066079565890253</v>
+        <v>0.77195167817096844</v>
       </c>
       <c r="E53">
         <f t="shared" si="1"/>
@@ -3418,7 +3423,7 @@
       </c>
       <c r="H53">
         <f t="shared" ca="1" si="4"/>
-        <v>0.12066079565890253</v>
+        <v>0.77195167817096844</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3434,7 +3439,7 @@
       </c>
       <c r="D54">
         <f ca="1"/>
-        <v>0.7402261013506376</v>
+        <v>0.15115754224852285</v>
       </c>
       <c r="E54">
         <f t="shared" si="1"/>
@@ -3450,7 +3455,7 @@
       </c>
       <c r="H54">
         <f t="shared" ca="1" si="4"/>
-        <v>0.7402261013506376</v>
+        <v>0.15115754224852285</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3466,7 +3471,7 @@
       </c>
       <c r="D55">
         <f ca="1"/>
-        <v>0.59840612245510938</v>
+        <v>0.1308136126154289</v>
       </c>
       <c r="E55">
         <f t="shared" si="1"/>
@@ -3482,7 +3487,7 @@
       </c>
       <c r="H55">
         <f t="shared" ca="1" si="4"/>
-        <v>0.59840612245510938</v>
+        <v>0.1308136126154289</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3498,7 +3503,7 @@
       </c>
       <c r="D56">
         <f ca="1"/>
-        <v>0.45218468174951487</v>
+        <v>0.52735043157173811</v>
       </c>
       <c r="E56">
         <f t="shared" si="1"/>
@@ -3514,7 +3519,7 @@
       </c>
       <c r="H56">
         <f t="shared" ca="1" si="4"/>
-        <v>0.45218468174951487</v>
+        <v>0.52735043157173811</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3530,7 +3535,7 @@
       </c>
       <c r="D57">
         <f ca="1"/>
-        <v>0.29656183889152232</v>
+        <v>0.7015579341649063</v>
       </c>
       <c r="E57">
         <f t="shared" si="1"/>
@@ -3546,7 +3551,7 @@
       </c>
       <c r="H57">
         <f t="shared" ca="1" si="4"/>
-        <v>0.29656183889152232</v>
+        <v>0.7015579341649063</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3562,7 +3567,7 @@
       </c>
       <c r="D58">
         <f ca="1"/>
-        <v>5.8034472312355367E-2</v>
+        <v>0.54241414212575956</v>
       </c>
       <c r="E58">
         <f t="shared" si="1"/>
@@ -3578,7 +3583,7 @@
       </c>
       <c r="H58">
         <f t="shared" ca="1" si="4"/>
-        <v>5.8034472312355367E-2</v>
+        <v>0.54241414212575956</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3594,7 +3599,7 @@
       </c>
       <c r="D59">
         <f ca="1"/>
-        <v>0.41385966026464172</v>
+        <v>0.15081201508931008</v>
       </c>
       <c r="E59">
         <f t="shared" si="1"/>
@@ -3610,7 +3615,7 @@
       </c>
       <c r="H59">
         <f t="shared" ca="1" si="4"/>
-        <v>2.4138596602646416</v>
+        <v>2.15081201508931</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3626,7 +3631,7 @@
       </c>
       <c r="D60">
         <f ca="1"/>
-        <v>0.30814424716914091</v>
+        <v>0.9782877681928569</v>
       </c>
       <c r="E60">
         <f t="shared" si="1"/>
@@ -3642,7 +3647,7 @@
       </c>
       <c r="H60">
         <f t="shared" ca="1" si="4"/>
-        <v>2.3081442471691407</v>
+        <v>2.9782877681928568</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3658,7 +3663,7 @@
       </c>
       <c r="D61">
         <f ca="1"/>
-        <v>0.70973446136805318</v>
+        <v>0.87755508165942753</v>
       </c>
       <c r="E61">
         <f t="shared" si="1"/>
@@ -3674,7 +3679,7 @@
       </c>
       <c r="H61">
         <f t="shared" ca="1" si="4"/>
-        <v>2.7097344613680532</v>
+        <v>2.8775550816594277</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3690,7 +3695,7 @@
       </c>
       <c r="D62">
         <f ca="1"/>
-        <v>0.97741617303624395</v>
+        <v>0.28663936592778794</v>
       </c>
       <c r="E62">
         <f t="shared" si="1"/>
@@ -3706,7 +3711,7 @@
       </c>
       <c r="H62">
         <f t="shared" ca="1" si="4"/>
-        <v>2.9774161730362438</v>
+        <v>2.2866393659277877</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3722,7 +3727,7 @@
       </c>
       <c r="D63">
         <f ca="1"/>
-        <v>0.83264751205207954</v>
+        <v>0.65621401644352273</v>
       </c>
       <c r="E63">
         <f t="shared" si="1"/>
@@ -3738,7 +3743,7 @@
       </c>
       <c r="H63">
         <f t="shared" ca="1" si="4"/>
-        <v>2.8326475120520795</v>
+        <v>2.6562140164435228</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3754,7 +3759,7 @@
       </c>
       <c r="D64">
         <f ca="1"/>
-        <v>0.68715754104674087</v>
+        <v>0.74370785736381406</v>
       </c>
       <c r="E64">
         <f t="shared" si="1"/>
@@ -3770,7 +3775,7 @@
       </c>
       <c r="H64">
         <f t="shared" ca="1" si="4"/>
-        <v>2.6871575410467408</v>
+        <v>2.7437078573638143</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3786,7 +3791,7 @@
       </c>
       <c r="D65">
         <f ca="1"/>
-        <v>0.33226130385307395</v>
+        <v>0.53034549461795277</v>
       </c>
       <c r="E65">
         <f t="shared" si="1"/>
@@ -3802,7 +3807,7 @@
       </c>
       <c r="H65">
         <f t="shared" ca="1" si="4"/>
-        <v>0.33226130385307395</v>
+        <v>0.53034549461795277</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3818,7 +3823,7 @@
       </c>
       <c r="D66">
         <f ca="1"/>
-        <v>0.96681640820509573</v>
+        <v>0.94533663534186496</v>
       </c>
       <c r="E66">
         <f t="shared" si="1"/>
@@ -3834,7 +3839,7 @@
       </c>
       <c r="H66">
         <f t="shared" ca="1" si="4"/>
-        <v>0.96681640820509573</v>
+        <v>0.94533663534186496</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3850,7 +3855,7 @@
       </c>
       <c r="D67">
         <f ca="1"/>
-        <v>0.93076280053761484</v>
+        <v>0.48250393374354528</v>
       </c>
       <c r="E67">
         <f t="shared" ref="E67:E73" si="6">IF(B67="Europe",1,0)</f>
@@ -3866,7 +3871,7 @@
       </c>
       <c r="H67">
         <f t="shared" ref="H67:H73" ca="1" si="9">SUM(D67:G67)</f>
-        <v>0.93076280053761484</v>
+        <v>0.48250393374354528</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3882,7 +3887,7 @@
       </c>
       <c r="D68">
         <f ca="1"/>
-        <v>5.1959462495823949E-2</v>
+        <v>0.21978252295276735</v>
       </c>
       <c r="E68">
         <f t="shared" si="6"/>
@@ -3898,7 +3903,7 @@
       </c>
       <c r="H68">
         <f t="shared" ca="1" si="9"/>
-        <v>5.1959462495823949E-2</v>
+        <v>0.21978252295276735</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3914,7 +3919,7 @@
       </c>
       <c r="D69">
         <f ca="1"/>
-        <v>0.92422374275418029</v>
+        <v>0.96040532516298127</v>
       </c>
       <c r="E69">
         <f t="shared" si="6"/>
@@ -3930,7 +3935,7 @@
       </c>
       <c r="H69">
         <f t="shared" ca="1" si="9"/>
-        <v>0.92422374275418029</v>
+        <v>0.96040532516298127</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3946,7 +3951,7 @@
       </c>
       <c r="D70">
         <f ca="1"/>
-        <v>0.56148099198997736</v>
+        <v>0.74185692114156843</v>
       </c>
       <c r="E70">
         <f t="shared" si="6"/>
@@ -3962,7 +3967,7 @@
       </c>
       <c r="H70">
         <f t="shared" ca="1" si="9"/>
-        <v>0.56148099198997736</v>
+        <v>0.74185692114156843</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -3978,7 +3983,7 @@
       </c>
       <c r="D71">
         <f ca="1"/>
-        <v>0.20323324392961417</v>
+        <v>0.87040305928696227</v>
       </c>
       <c r="E71">
         <f t="shared" si="6"/>
@@ -3994,7 +3999,7 @@
       </c>
       <c r="H71">
         <f t="shared" ca="1" si="9"/>
-        <v>2.2032332439296143</v>
+        <v>2.8704030592869625</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -4010,7 +4015,7 @@
       </c>
       <c r="D72">
         <f ca="1"/>
-        <v>0.75041547329288993</v>
+        <v>0.11549437565934129</v>
       </c>
       <c r="E72">
         <f t="shared" si="6"/>
@@ -4026,7 +4031,7 @@
       </c>
       <c r="H72">
         <f t="shared" ca="1" si="9"/>
-        <v>2.75041547329289</v>
+        <v>2.1154943756593414</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -4042,7 +4047,7 @@
       </c>
       <c r="D73">
         <f ca="1"/>
-        <v>0.33558318044499902</v>
+        <v>0.39726452337150553</v>
       </c>
       <c r="E73">
         <f t="shared" si="6"/>
@@ -4058,7 +4063,7 @@
       </c>
       <c r="H73">
         <f t="shared" ca="1" si="9"/>
-        <v>2.3355831804449991</v>
+        <v>2.3972645233715055</v>
       </c>
     </row>
   </sheetData>

</xml_diff>